<commit_message>
feat: importacion masiva terminada
</commit_message>
<xml_diff>
--- a/frontend/public/modelos/productos.xlsx
+++ b/frontend/public/modelos/productos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\ProyectoSAAS\frontend\public\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD20950-1E49-4AFC-B575-FE778BEC1A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F87881C-B92D-4B29-887B-F98F32195252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,19 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Nombre del producto (obligatorio)</t>
-  </si>
-  <si>
-    <t>Precio de compra (número, obligatorio)</t>
-  </si>
-  <si>
-    <t>Precio de venta (número, obligatorio)</t>
-  </si>
-  <si>
-    <t>ID de la categoría (opcional)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>nombre</t>
   </si>
@@ -53,28 +41,28 @@
     <t>precioCompra</t>
   </si>
   <si>
+    <t>categoriaId</t>
+  </si>
+  <si>
+    <t>cuchillo tramontina #5 22902/005</t>
+  </si>
+  <si>
+    <t>cuchillo tramontina #5 22902/006</t>
+  </si>
+  <si>
+    <t>cuchillo tramontina #5 22902/007</t>
+  </si>
+  <si>
+    <t>cuchillo tramontina #5 22902/008</t>
+  </si>
+  <si>
+    <t>cuchillo tramontina #5 22902/009</t>
+  </si>
+  <si>
+    <t>6b6ebab0-e993-4da1-be42-69e7ad208af0</t>
+  </si>
+  <si>
     <t>precioVenta</t>
-  </si>
-  <si>
-    <t>categoriaId</t>
-  </si>
-  <si>
-    <t>cuchillo tramontina #5 22902/005</t>
-  </si>
-  <si>
-    <t>cuchillo tramontina #5 22902/006</t>
-  </si>
-  <si>
-    <t>cuchillo tramontina #5 22902/007</t>
-  </si>
-  <si>
-    <t>cuchillo tramontina #5 22902/008</t>
-  </si>
-  <si>
-    <t>cuchillo tramontina #5 22902/009</t>
-  </si>
-  <si>
-    <t>6b6ebab0-e993-4da1-be42-69e7ad208af0</t>
   </si>
 </sst>
 </file>
@@ -91,17 +79,19 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,10 +119,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,18 +423,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,103 +445,83 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>45000</v>
+      </c>
+      <c r="C2">
+        <f>+B2+B2*50%</f>
+        <v>67500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3">
+        <v>55000</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="0">+B3+B3*50%</f>
+        <v>82500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>45000</v>
-      </c>
-      <c r="C3">
-        <f>+B3+B3*50%</f>
-        <v>67500</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
       <c r="B4">
-        <v>55000</v>
+        <v>65000</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C7" si="0">+B4+B4*50%</f>
-        <v>82500</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>65000</v>
-      </c>
-      <c r="C5">
         <f t="shared" si="0"/>
         <v>97500</v>
       </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>75000</v>
+      </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>75000</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>112500</v>
+        <v>85000</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>85000</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>127500</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>